<commit_message>
fix: fix functionalities of RES-002
</commit_message>
<xml_diff>
--- a/excels/generic-excel.xlsx
+++ b/excels/generic-excel.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vicen_fpn6\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\Workspace\PhP Projects\Proyecto_Turjoy_IS\excels\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B15B6ABA-1434-42EE-959C-7D0B507F97B6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A6AB53EA-4B61-4C10-AEF7-EB6D183FEF9B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{2A3673FA-9B1B-4E8E-8FB4-EBD7DDB24E7A}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{2A3673FA-9B1B-4E8E-8FB4-EBD7DDB24E7A}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -73,8 +73,8 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
-    <numFmt numFmtId="6" formatCode="&quot;$&quot;#,##0;[Red]&quot;$&quot;\-#,##0"/>
-    <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0"/>
+    <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0;[Red]&quot;$&quot;\-#,##0"/>
+    <numFmt numFmtId="165" formatCode="&quot;$&quot;#,##0"/>
   </numFmts>
   <fonts count="4" x14ac:knownFonts="1">
     <font>
@@ -132,8 +132,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1"/>
-    <xf numFmtId="6" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hipervínculo" xfId="1" builtinId="8"/>
@@ -452,15 +452,15 @@
   <dimension ref="A1:E8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H17" sqref="H17"/>
+      <selection activeCell="D8" sqref="A4:D8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="18.109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -474,7 +474,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -485,7 +485,7 @@
         <v>5000</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -499,7 +499,7 @@
         <v>12000</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>5</v>
       </c>
@@ -512,7 +512,7 @@
       <c r="D4" s="4"/>
       <c r="E4" s="1"/>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>2</v>
       </c>
@@ -526,7 +526,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>7</v>
       </c>
@@ -541,7 +541,7 @@
       </c>
       <c r="E6" s="1"/>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>5</v>
       </c>
@@ -556,7 +556,7 @@
       </c>
       <c r="E7" s="1"/>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
         <v>6</v>
       </c>

</xml_diff>